<commit_message>
double check and nothing chance
</commit_message>
<xml_diff>
--- a/Test_Case_Template.xlsx
+++ b/Test_Case_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duong Van Tra\OneDrive\Tài liệu\GitHub\Kiem-Thu-phan-mem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4992FE-18C7-4774-998B-C9A3F1365629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E647161-D264-48AE-8938-7FE12B9176A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="801" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1634,9 +1634,6 @@
     <t>Giao diện hiển thị tốt trên nhiều trình duyệt</t>
   </si>
   <si>
-    <t>Website hiển thị giống với các trình duyệt khác</t>
-  </si>
-  <si>
     <t>Website hiển thị đồng nhất ở mọi trình duyệt phổ biến</t>
   </si>
   <si>
@@ -1762,9 +1759,6 @@
     <t>Quản lý ID tài khoản người dùng tốt</t>
   </si>
   <si>
-    <t>ID sản phẩm phải riên lẻ và được sắp xếp tốt</t>
-  </si>
-  <si>
     <t>Người dùng đã có tài khoản chọn "Mua" hoặc "Trả góp" sản phẩm có số lượng bằng 0</t>
   </si>
   <si>
@@ -1817,6 +1811,12 @@
   </si>
   <si>
     <t>Mọi tài khoản được tạo phải khả dụng</t>
+  </si>
+  <si>
+    <t>ID sản phẩm phải riêng lẻ và được sắp xếp tốt</t>
+  </si>
+  <si>
+    <t>Website hiển thị chính xác và đầy đủ các chức năng giống với các trình duyệt khác</t>
   </si>
 </sst>
 </file>
@@ -2139,7 +2139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2332,83 +2332,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2421,10 +2352,103 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2433,140 +2457,161 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -2577,85 +2622,46 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -2669,12 +2675,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2683,6 +2683,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3164,54 +3170,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
+      <c r="A1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
     </row>
     <row r="3" spans="1:16" s="3" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="96"/>
-      <c r="P4" s="96"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
     </row>
     <row r="5" spans="1:16" s="3" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="96"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P6"/>
@@ -3222,30 +3228,30 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:16" s="5" customFormat="1" ht="23" x14ac:dyDescent="0.5">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="95"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
     </row>
     <row r="11" spans="1:16" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="F11" s="6"/>
@@ -3263,272 +3269,272 @@
     </row>
     <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="93"/>
-      <c r="N13" s="93"/>
-      <c r="O13" s="93"/>
-      <c r="P13" s="93"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="69"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="69"/>
     </row>
     <row r="14" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80" t="s">
+      <c r="C14" s="70"/>
+      <c r="D14" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80" t="s">
+      <c r="E14" s="70"/>
+      <c r="F14" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80" t="s">
+      <c r="G14" s="70"/>
+      <c r="H14" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80" t="s">
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="80"/>
-      <c r="M14" s="80"/>
-      <c r="N14" s="80" t="s">
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
+      <c r="N14" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="O14" s="80"/>
-      <c r="P14" s="80"/>
+      <c r="O14" s="70"/>
+      <c r="P14" s="70"/>
     </row>
     <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.25">
       <c r="B15" s="97">
         <v>45833</v>
       </c>
       <c r="C15" s="97"/>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="71"/>
+      <c r="E15" s="94"/>
       <c r="F15" s="74" t="s">
+        <v>199</v>
+      </c>
+      <c r="G15" s="74"/>
+      <c r="H15" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="96" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75"/>
+    </row>
+    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+      <c r="B16" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+    </row>
+    <row r="17" spans="2:13" ht="13" x14ac:dyDescent="0.3">
+      <c r="B17" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
+    </row>
+    <row r="18" spans="2:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="B18" s="78">
+        <v>45833</v>
+      </c>
+      <c r="C18" s="79"/>
+      <c r="D18" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="94"/>
+      <c r="F18" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="G15" s="74"/>
-      <c r="H15" s="75" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="76"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="76"/>
-    </row>
-    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.3">
-      <c r="B16" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="89"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="89"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="89"/>
-      <c r="M16" s="89"/>
-    </row>
-    <row r="17" spans="2:13" ht="13" x14ac:dyDescent="0.3">
-      <c r="B17" s="80" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="80"/>
-      <c r="M17" s="80"/>
-    </row>
-    <row r="18" spans="2:13" ht="13" x14ac:dyDescent="0.25">
-      <c r="B18" s="84">
-        <v>45833</v>
-      </c>
-      <c r="C18" s="85"/>
-      <c r="D18" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="71"/>
-      <c r="F18" s="72" t="s">
+      <c r="G18" s="84"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="75" t="s">
-        <v>202</v>
-      </c>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
     </row>
     <row r="19" spans="2:13" ht="13" x14ac:dyDescent="0.25">
-      <c r="B19" s="84"/>
-      <c r="C19" s="85"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="79"/>
       <c r="D19" s="74"/>
       <c r="E19" s="74"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="87"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="88"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="83"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="85"/>
     </row>
     <row r="20" spans="2:13" ht="13" x14ac:dyDescent="0.25">
-      <c r="B20" s="84"/>
-      <c r="C20" s="85"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="79"/>
       <c r="D20" s="74"/>
       <c r="E20" s="74"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="87"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="88"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="83"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="85"/>
     </row>
     <row r="21" spans="2:13" ht="13" x14ac:dyDescent="0.25">
-      <c r="B21" s="84"/>
-      <c r="C21" s="85"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="79"/>
       <c r="D21" s="74"/>
       <c r="E21" s="74"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="87"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="88"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="84"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="85"/>
     </row>
     <row r="22" spans="2:13" ht="13" x14ac:dyDescent="0.25">
-      <c r="B22" s="84"/>
-      <c r="C22" s="85"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="79"/>
       <c r="D22" s="74"/>
       <c r="E22" s="74"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="88"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="85"/>
     </row>
     <row r="23" spans="2:13" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="B23" s="91" t="s">
+      <c r="B23" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91" t="s">
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91" t="s">
+      <c r="F23" s="89"/>
+      <c r="G23" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="91"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="91"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="91"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="89"/>
     </row>
     <row r="24" spans="2:13" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="B24" s="81" t="s">
+      <c r="B24" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="81" t="s">
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="J24" s="83"/>
-      <c r="K24" s="81" t="s">
+      <c r="J24" s="82"/>
+      <c r="K24" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="L24" s="82"/>
-      <c r="M24" s="83"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="82"/>
     </row>
     <row r="25" spans="2:13" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="B25" s="77"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="68"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="87"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="87"/>
     </row>
     <row r="26" spans="2:13" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="B26" s="77"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="70"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="88"/>
+      <c r="M26" s="87"/>
     </row>
     <row r="27" spans="2:13" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
       <c r="I27" s="74"/>
       <c r="J27" s="74"/>
       <c r="K27" s="74"/>
@@ -3536,87 +3542,87 @@
       <c r="M27" s="74"/>
     </row>
     <row r="28" spans="2:13" ht="13" x14ac:dyDescent="0.3">
-      <c r="B28" s="90" t="s">
+      <c r="B28" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="77"/>
+      <c r="M28" s="77"/>
     </row>
     <row r="29" spans="2:13" ht="13" x14ac:dyDescent="0.3">
-      <c r="B29" s="80" t="s">
+      <c r="B29" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="80"/>
-      <c r="D29" s="80" t="s">
+      <c r="C29" s="70"/>
+      <c r="D29" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80" t="s">
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="80"/>
+      <c r="H29" s="70"/>
     </row>
     <row r="30" spans="2:13" ht="13" x14ac:dyDescent="0.25">
-      <c r="B30" s="84"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="88"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="84"/>
+      <c r="F30" s="85"/>
       <c r="G30" s="74"/>
       <c r="H30" s="74"/>
     </row>
     <row r="31" spans="2:13" ht="13" x14ac:dyDescent="0.25">
-      <c r="B31" s="84"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="88"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="85"/>
       <c r="G31" s="74"/>
       <c r="H31" s="74"/>
     </row>
     <row r="32" spans="2:13" ht="13" x14ac:dyDescent="0.25">
-      <c r="B32" s="84"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="88"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="85"/>
       <c r="G32" s="74"/>
       <c r="H32" s="74"/>
     </row>
     <row r="33" spans="2:8" ht="13" x14ac:dyDescent="0.25">
-      <c r="B33" s="84"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="88"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="85"/>
       <c r="G33" s="74"/>
       <c r="H33" s="74"/>
     </row>
     <row r="34" spans="2:8" ht="13" x14ac:dyDescent="0.25">
-      <c r="B34" s="84"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="88"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="85"/>
       <c r="G34" s="74"/>
       <c r="H34" s="74"/>
     </row>
     <row r="35" spans="2:8" ht="13" x14ac:dyDescent="0.25">
-      <c r="B35" s="84"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="88"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="85"/>
       <c r="G35" s="74"/>
       <c r="H35" s="74"/>
     </row>
@@ -3628,16 +3634,57 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="A1:E5"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="F9:K9"/>
-    <mergeCell ref="E10:L10"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="N1:P5"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="N15:P15"/>
@@ -3654,57 +3701,16 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="K24:M24"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="A1:E5"/>
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="F9:K9"/>
+    <mergeCell ref="E10:L10"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="N1:P5"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:J14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3718,9 +3724,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I43" sqref="I43:I46"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3738,17 +3744,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" x14ac:dyDescent="0.5">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -3832,35 +3838,35 @@
     </row>
     <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="125" t="s">
+      <c r="D7" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="141" t="s">
+      <c r="E7" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="142"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="125" t="s">
+      <c r="F7" s="121"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="125" t="s">
+      <c r="I7" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="125" t="s">
+      <c r="J7" s="118" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
       <c r="E8" s="17" t="s">
         <v>20</v>
       </c>
@@ -3870,19 +3876,19 @@
       <c r="G8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
     </row>
     <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="144" t="s">
+      <c r="D9" s="103" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="19" t="s">
@@ -3894,19 +3900,19 @@
       <c r="G9" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="98" t="s">
+      <c r="H9" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="171" t="s">
+      <c r="I9" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="127"/>
+      <c r="J9" s="128"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="108"/>
-      <c r="C10" s="113"/>
-      <c r="D10" s="145"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="104"/>
       <c r="E10" s="21" t="s">
         <v>37</v>
       </c>
@@ -3916,15 +3922,15 @@
       <c r="G10" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="99"/>
-      <c r="I10" s="172"/>
-      <c r="J10" s="124"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="129"/>
     </row>
     <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="108"/>
-      <c r="C11" s="113"/>
-      <c r="D11" s="145"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="104"/>
       <c r="E11" s="21" t="s">
         <v>38</v>
       </c>
@@ -3934,15 +3940,15 @@
       <c r="G11" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="99"/>
-      <c r="I11" s="172"/>
-      <c r="J11" s="124"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="129"/>
     </row>
     <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
-      <c r="B12" s="108"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="145"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="21" t="s">
         <v>161</v>
       </c>
@@ -3952,15 +3958,15 @@
       <c r="G12" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="99"/>
-      <c r="I12" s="172"/>
-      <c r="J12" s="124"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="124"/>
+      <c r="J12" s="129"/>
     </row>
     <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="108"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="145"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="104"/>
       <c r="E13" s="21" t="s">
         <v>42</v>
       </c>
@@ -3970,15 +3976,15 @@
       <c r="G13" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="99"/>
-      <c r="I13" s="172"/>
-      <c r="J13" s="124"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="129"/>
     </row>
     <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="108"/>
-      <c r="C14" s="113"/>
-      <c r="D14" s="145"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="104"/>
       <c r="E14" s="21" t="s">
         <v>40</v>
       </c>
@@ -3988,15 +3994,15 @@
       <c r="G14" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="99"/>
-      <c r="I14" s="172"/>
-      <c r="J14" s="124"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="124"/>
+      <c r="J14" s="129"/>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="108"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="146"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="105"/>
       <c r="E15" s="21" t="s">
         <v>43</v>
       </c>
@@ -4006,17 +4012,17 @@
       <c r="G15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="100"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="124"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="125"/>
+      <c r="J15" s="129"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="108"/>
-      <c r="C16" s="112" t="s">
+      <c r="B16" s="99"/>
+      <c r="C16" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="109" t="s">
+      <c r="D16" s="113" t="s">
         <v>49</v>
       </c>
       <c r="E16" s="19" t="s">
@@ -4028,19 +4034,19 @@
       <c r="G16" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="98" t="s">
+      <c r="H16" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="171" t="s">
+      <c r="I16" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="J16" s="124"/>
+      <c r="J16" s="129"/>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="108"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="110"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="114"/>
       <c r="E17" s="24" t="s">
         <v>42</v>
       </c>
@@ -4050,15 +4056,15 @@
       <c r="G17" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="99"/>
-      <c r="I17" s="172"/>
-      <c r="J17" s="124"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="129"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="108"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="110"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="114"/>
       <c r="E18" s="21" t="s">
         <v>40</v>
       </c>
@@ -4068,15 +4074,15 @@
       <c r="G18" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H18" s="99"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="124"/>
+      <c r="H18" s="107"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="129"/>
     </row>
     <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="108"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="111"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="115"/>
       <c r="E19" s="21" t="s">
         <v>43</v>
       </c>
@@ -4086,13 +4092,13 @@
       <c r="G19" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="100"/>
-      <c r="I19" s="173"/>
-      <c r="J19" s="124"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="129"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="108"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="9" t="s">
         <v>50</v>
       </c>
@@ -4117,53 +4123,53 @@
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="112" t="s">
+      <c r="C21" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="109" t="s">
+      <c r="D21" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="98" t="s">
+      <c r="E21" s="106" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="98" t="s">
+      <c r="F21" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="G21" s="112" t="s">
+      <c r="G21" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="H21" s="98" t="s">
+      <c r="H21" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="I21" s="138" t="s">
+      <c r="I21" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="128" t="s">
+      <c r="J21" s="130" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" s="108"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="100"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="114"/>
-      <c r="H22" s="100"/>
-      <c r="I22" s="139"/>
-      <c r="J22" s="129"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="108"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="108"/>
+      <c r="I22" s="127"/>
+      <c r="J22" s="131"/>
     </row>
     <row r="23" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
-      <c r="B23" s="108"/>
-      <c r="C23" s="112" t="s">
+      <c r="B23" s="99"/>
+      <c r="C23" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="109" t="s">
+      <c r="D23" s="113" t="s">
         <v>62</v>
       </c>
       <c r="E23" s="19" t="s">
@@ -4175,19 +4181,19 @@
       <c r="G23" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="98" t="s">
+      <c r="H23" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="I23" s="171" t="s">
+      <c r="I23" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="J23" s="124"/>
+      <c r="J23" s="129"/>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
-      <c r="B24" s="108"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="110"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="114"/>
       <c r="E24" s="21" t="s">
         <v>67</v>
       </c>
@@ -4197,16 +4203,16 @@
       <c r="G24" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="99"/>
-      <c r="I24" s="172"/>
-      <c r="J24" s="124"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="124"/>
+      <c r="J24" s="129"/>
     </row>
     <row r="25" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
-      <c r="B25" s="108"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="99" t="s">
+      <c r="B25" s="99"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="107" t="s">
         <v>69</v>
       </c>
       <c r="F25" s="22" t="s">
@@ -4215,31 +4221,31 @@
       <c r="G25" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="99"/>
-      <c r="I25" s="172"/>
-      <c r="J25" s="124"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="124"/>
+      <c r="J25" s="129"/>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
-      <c r="B26" s="108"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="110"/>
-      <c r="E26" s="99"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="114"/>
+      <c r="E26" s="107"/>
       <c r="F26" s="22" t="s">
         <v>146</v>
       </c>
       <c r="G26" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="99"/>
-      <c r="I26" s="172"/>
-      <c r="J26" s="124"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="129"/>
     </row>
     <row r="27" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
-      <c r="B27" s="108"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="111"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="115"/>
       <c r="E27" s="21" t="s">
         <v>61</v>
       </c>
@@ -4249,75 +4255,75 @@
       <c r="G27" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="100"/>
-      <c r="I27" s="173"/>
-      <c r="J27" s="124"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="125"/>
+      <c r="J27" s="129"/>
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
-      <c r="B28" s="108"/>
-      <c r="C28" s="112" t="s">
+      <c r="B28" s="99"/>
+      <c r="C28" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="118" t="s">
+      <c r="D28" s="141" t="s">
         <v>72</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="26" t="s">
         <v>73</v>
       </c>
       <c r="G28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H28" s="98" t="s">
+      <c r="H28" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="I28" s="171" t="s">
+      <c r="I28" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="J28" s="124"/>
+      <c r="J28" s="129"/>
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
-      <c r="B29" s="108"/>
-      <c r="C29" s="113"/>
-      <c r="D29" s="170"/>
-      <c r="E29" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>216</v>
+      <c r="B29" s="99"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="142"/>
+      <c r="E29" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>214</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="99"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="124"/>
+      <c r="H29" s="107"/>
+      <c r="I29" s="124"/>
+      <c r="J29" s="129"/>
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
-      <c r="B30" s="108"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="119"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="102"/>
+      <c r="D30" s="143"/>
       <c r="E30" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="29" t="s">
         <v>147</v>
       </c>
       <c r="G30" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H30" s="100"/>
-      <c r="I30" s="173"/>
-      <c r="J30" s="124"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="125"/>
+      <c r="J30" s="129"/>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
-      <c r="B31" s="104"/>
+      <c r="B31" s="112"/>
       <c r="C31" s="9" t="s">
         <v>104</v>
       </c>
@@ -4342,51 +4348,51 @@
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
-      <c r="B32" s="103" t="s">
+      <c r="B32" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="121" t="s">
+      <c r="C32" s="110" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="109" t="s">
+      <c r="D32" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="98" t="s">
+      <c r="E32" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="131" t="s">
+      <c r="F32" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="G32" s="132" t="s">
+      <c r="G32" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="H32" s="131" t="s">
+      <c r="H32" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="I32" s="130" t="s">
+      <c r="I32" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="J32" s="124"/>
+      <c r="J32" s="129"/>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
-      <c r="B33" s="108"/>
-      <c r="C33" s="123"/>
-      <c r="D33" s="111"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="131"/>
-      <c r="G33" s="112"/>
-      <c r="H33" s="131"/>
-      <c r="I33" s="130"/>
-      <c r="J33" s="124"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="132"/>
+      <c r="J33" s="129"/>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
-      <c r="B34" s="108"/>
-      <c r="C34" s="121" t="s">
+      <c r="B34" s="99"/>
+      <c r="C34" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="109" t="s">
+      <c r="D34" s="113" t="s">
         <v>59</v>
       </c>
       <c r="E34" s="19" t="s">
@@ -4398,19 +4404,19 @@
       <c r="G34" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="136" t="s">
+      <c r="H34" s="137" t="s">
         <v>95</v>
       </c>
-      <c r="I34" s="116" t="s">
+      <c r="I34" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="J34" s="124"/>
+      <c r="J34" s="129"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
-      <c r="B35" s="108"/>
-      <c r="C35" s="122"/>
-      <c r="D35" s="110"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="116"/>
+      <c r="D35" s="114"/>
       <c r="E35" s="21" t="s">
         <v>79</v>
       </c>
@@ -4420,15 +4426,15 @@
       <c r="G35" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H35" s="136"/>
-      <c r="I35" s="116"/>
-      <c r="J35" s="124"/>
+      <c r="H35" s="137"/>
+      <c r="I35" s="139"/>
+      <c r="J35" s="129"/>
     </row>
     <row r="36" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-      <c r="B36" s="108"/>
-      <c r="C36" s="123"/>
-      <c r="D36" s="111"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="111"/>
+      <c r="D36" s="115"/>
       <c r="E36" s="23" t="s">
         <v>81</v>
       </c>
@@ -4438,17 +4444,17 @@
       <c r="G36" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H36" s="137"/>
-      <c r="I36" s="117"/>
-      <c r="J36" s="124"/>
+      <c r="H36" s="138"/>
+      <c r="I36" s="140"/>
+      <c r="J36" s="129"/>
     </row>
     <row r="37" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
-      <c r="B37" s="108"/>
-      <c r="C37" s="121" t="s">
+      <c r="B37" s="99"/>
+      <c r="C37" s="110" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="109" t="s">
+      <c r="D37" s="113" t="s">
         <v>84</v>
       </c>
       <c r="E37" s="21" t="s">
@@ -4460,19 +4466,19 @@
       <c r="G37" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="98" t="s">
+      <c r="H37" s="106" t="s">
         <v>90</v>
       </c>
-      <c r="I37" s="133" t="s">
+      <c r="I37" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="J37" s="124"/>
+      <c r="J37" s="129"/>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
-      <c r="B38" s="108"/>
-      <c r="C38" s="122"/>
-      <c r="D38" s="110"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="114"/>
       <c r="E38" s="21" t="s">
         <v>87</v>
       </c>
@@ -4482,15 +4488,15 @@
       <c r="G38" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="H38" s="99"/>
-      <c r="I38" s="134"/>
-      <c r="J38" s="124"/>
+      <c r="H38" s="107"/>
+      <c r="I38" s="135"/>
+      <c r="J38" s="129"/>
     </row>
     <row r="39" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
-      <c r="B39" s="108"/>
-      <c r="C39" s="123"/>
-      <c r="D39" s="111"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="111"/>
+      <c r="D39" s="115"/>
       <c r="E39" s="23" t="s">
         <v>86</v>
       </c>
@@ -4500,13 +4506,13 @@
       <c r="G39" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="100"/>
-      <c r="I39" s="135"/>
-      <c r="J39" s="124"/>
+      <c r="H39" s="108"/>
+      <c r="I39" s="136"/>
+      <c r="J39" s="129"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
-      <c r="B40" s="104"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="34" t="s">
         <v>91</v>
       </c>
@@ -4531,13 +4537,13 @@
     </row>
     <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
-      <c r="B41" s="103" t="s">
+      <c r="B41" s="98" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="98" t="s">
+      <c r="C41" s="106" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="98" t="s">
+      <c r="D41" s="106" t="s">
         <v>153</v>
       </c>
       <c r="E41" s="19" t="s">
@@ -4549,18 +4555,18 @@
       <c r="G41" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="98" t="s">
+      <c r="H41" s="106" t="s">
         <v>155</v>
       </c>
-      <c r="I41" s="101" t="s">
+      <c r="I41" s="151" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
-      <c r="B42" s="104"/>
-      <c r="C42" s="100"/>
-      <c r="D42" s="100"/>
+      <c r="B42" s="112"/>
+      <c r="C42" s="108"/>
+      <c r="D42" s="108"/>
       <c r="E42" s="21" t="s">
         <v>152</v>
       </c>
@@ -4570,18 +4576,18 @@
       <c r="G42" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H42" s="120"/>
-      <c r="I42" s="102"/>
+      <c r="H42" s="150"/>
+      <c r="I42" s="152"/>
     </row>
     <row r="43" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
-      <c r="B43" s="103" t="s">
+      <c r="B43" s="98" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="105" t="s">
+      <c r="C43" s="147" t="s">
         <v>156</v>
       </c>
-      <c r="D43" s="98" t="s">
+      <c r="D43" s="106" t="s">
         <v>157</v>
       </c>
       <c r="E43" s="19" t="s">
@@ -4593,18 +4599,18 @@
       <c r="G43" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H43" s="98" t="s">
+      <c r="H43" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="I43" s="174" t="s">
+      <c r="I43" s="144" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
-      <c r="B44" s="108"/>
-      <c r="C44" s="106"/>
-      <c r="D44" s="99"/>
+      <c r="B44" s="99"/>
+      <c r="C44" s="148"/>
+      <c r="D44" s="107"/>
       <c r="E44" s="21" t="s">
         <v>159</v>
       </c>
@@ -4614,14 +4620,14 @@
       <c r="G44" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="99"/>
-      <c r="I44" s="175"/>
+      <c r="H44" s="107"/>
+      <c r="I44" s="145"/>
     </row>
     <row r="45" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
-      <c r="B45" s="108"/>
-      <c r="C45" s="106"/>
-      <c r="D45" s="99"/>
+      <c r="B45" s="99"/>
+      <c r="C45" s="148"/>
+      <c r="D45" s="107"/>
       <c r="E45" s="21" t="s">
         <v>160</v>
       </c>
@@ -4631,13 +4637,13 @@
       <c r="G45" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H45" s="99"/>
-      <c r="I45" s="175"/>
+      <c r="H45" s="107"/>
+      <c r="I45" s="145"/>
     </row>
     <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="104"/>
-      <c r="C46" s="107"/>
-      <c r="D46" s="100"/>
+      <c r="B46" s="112"/>
+      <c r="C46" s="149"/>
+      <c r="D46" s="108"/>
       <c r="E46" s="23" t="s">
         <v>163</v>
       </c>
@@ -4647,8 +4653,8 @@
       <c r="G46" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H46" s="100"/>
-      <c r="I46" s="176"/>
+      <c r="H46" s="108"/>
+      <c r="I46" s="146"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="58"/>
@@ -4752,6 +4758,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="I43:I46"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="J23:J27"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="I9:I15"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="C9:C15"/>
     <mergeCell ref="D9:D15"/>
@@ -4768,58 +4826,6 @@
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="I9:I15"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="J23:J27"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="I43:I46"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="C41:C42"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
@@ -4839,7 +4845,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E20"/>
+      <selection activeCell="E15" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4856,17 +4862,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" x14ac:dyDescent="0.5">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -4896,7 +4902,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="35">
-        <f>COUNTIF($I$12:$I$2016, "Failed")</f>
+        <f>COUNTIF($I$9:$I$2016, "Failed")</f>
         <v>4</v>
       </c>
     </row>
@@ -4912,7 +4918,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="35">
-        <f>COUNTIF($I$12:$I$2016, "Not Run")</f>
+        <f>COUNTIF($I$9:$I$2016, "Not Run")</f>
         <v>0</v>
       </c>
     </row>
@@ -4928,7 +4934,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="35">
-        <f>COUNTIF($I$12:$I$2016, "Not Completed")</f>
+        <f>COUNTIF($I$9:$I$2016, "Not Completed")</f>
         <v>0</v>
       </c>
     </row>
@@ -4944,41 +4950,41 @@
         <v>29</v>
       </c>
       <c r="I6" s="35">
-        <f>COUNTA(C11:C2015)</f>
-        <v>6</v>
+        <f>COUNTA(C9:C2015)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="125" t="s">
+      <c r="D7" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="141" t="s">
+      <c r="E7" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="142"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="125" t="s">
+      <c r="F7" s="121"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="125" t="s">
+      <c r="I7" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="125" t="s">
+      <c r="J7" s="118" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
+      <c r="B8" s="159"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="159"/>
       <c r="E8" s="17" t="s">
         <v>20</v>
       </c>
@@ -4988,19 +4994,19 @@
       <c r="G8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="159"/>
+      <c r="J8" s="159"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="161" t="s">
+      <c r="C9" s="157" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="160" t="s">
+      <c r="D9" s="155" t="s">
         <v>109</v>
       </c>
       <c r="E9" s="19" t="s">
@@ -5012,19 +5018,19 @@
       <c r="G9" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="150" t="s">
+      <c r="H9" s="156" t="s">
         <v>110</v>
       </c>
-      <c r="I9" s="115" t="s">
+      <c r="I9" s="161" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="124"/>
+      <c r="J9" s="129"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="108"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="150"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="158"/>
+      <c r="D10" s="156"/>
       <c r="E10" s="21" t="s">
         <v>138</v>
       </c>
@@ -5034,13 +5040,13 @@
       <c r="G10" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="151"/>
-      <c r="I10" s="117"/>
-      <c r="J10" s="124"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="140"/>
+      <c r="J10" s="129"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="104"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="34" t="s">
         <v>103</v>
       </c>
@@ -5092,13 +5098,13 @@
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="163" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="152" t="s">
+      <c r="C13" s="165" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="157" t="s">
+      <c r="D13" s="167" t="s">
         <v>99</v>
       </c>
       <c r="E13" s="19" t="s">
@@ -5110,19 +5116,19 @@
       <c r="G13" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="105" t="s">
+      <c r="H13" s="147" t="s">
         <v>116</v>
       </c>
-      <c r="I13" s="158" t="s">
+      <c r="I13" s="153" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="124"/>
+      <c r="J13" s="129"/>
     </row>
     <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="148"/>
-      <c r="C14" s="153"/>
-      <c r="D14" s="157"/>
+      <c r="B14" s="163"/>
+      <c r="C14" s="166"/>
+      <c r="D14" s="167"/>
       <c r="E14" s="23" t="s">
         <v>101</v>
       </c>
@@ -5132,19 +5138,19 @@
       <c r="G14" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="107"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="124"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="129"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="149" t="s">
+      <c r="B15" s="164" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="121" t="s">
+      <c r="C15" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="147" t="s">
+      <c r="D15" s="162" t="s">
         <v>122</v>
       </c>
       <c r="E15" s="21" t="s">
@@ -5156,21 +5162,21 @@
       <c r="G15" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="150" t="s">
+      <c r="H15" s="156" t="s">
         <v>127</v>
       </c>
-      <c r="I15" s="138" t="s">
+      <c r="I15" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="J15" s="128" t="s">
+      <c r="J15" s="130" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="149"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="147"/>
+      <c r="B16" s="164"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="162"/>
       <c r="E16" s="23" t="s">
         <v>124</v>
       </c>
@@ -5180,91 +5186,91 @@
       <c r="G16" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H16" s="151"/>
-      <c r="I16" s="139"/>
-      <c r="J16" s="129"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="131"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="98" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="110" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="106" t="s">
         <v>211</v>
       </c>
-      <c r="C17" s="121" t="s">
-        <v>209</v>
-      </c>
-      <c r="D17" s="98" t="s">
-        <v>212</v>
-      </c>
-      <c r="E17" s="98" t="s">
+      <c r="E17" s="106" t="s">
+        <v>202</v>
+      </c>
+      <c r="F17" s="22" t="s">
         <v>203</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>204</v>
       </c>
       <c r="G17" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="98" t="s">
-        <v>214</v>
-      </c>
-      <c r="I17" s="158" t="s">
+      <c r="H17" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="I17" s="153" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="108"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="107"/>
+      <c r="E18" s="107"/>
       <c r="F18" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G18" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="100"/>
-      <c r="I18" s="159"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="154"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="108"/>
-      <c r="C19" s="121" t="s">
-        <v>210</v>
-      </c>
-      <c r="D19" s="98" t="s">
-        <v>213</v>
-      </c>
-      <c r="E19" s="98" t="s">
+      <c r="B19" s="99"/>
+      <c r="C19" s="110" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="106" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="F19" s="20" t="s">
         <v>206</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>207</v>
       </c>
       <c r="G19" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="98" t="s">
-        <v>214</v>
-      </c>
-      <c r="I19" s="158" t="s">
+      <c r="H19" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="I19" s="153" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="111"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G20" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="100"/>
-      <c r="I20" s="159"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="154"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
@@ -5565,6 +5571,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="I19:I20"/>
@@ -5579,29 +5606,8 @@
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I15 I23:I24 I26 I29 I17 I32:I48 I19 I9 I11:I13" xr:uid="{2EEFFE48-0949-4D00-ABE5-F13E31C6E209}">
@@ -5618,7 +5624,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H7" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5635,17 +5641,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" x14ac:dyDescent="0.5">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="117" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -5659,8 +5665,8 @@
         <v>1</v>
       </c>
       <c r="I2" s="35">
-        <f>COUNTIF($I$13:$I$2017, "Passed")</f>
-        <v>1</v>
+        <f>COUNTIF($I$9:$I$2017, "Passed")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.3">
@@ -5675,7 +5681,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="35">
-        <f>COUNTIF($I$13:$I$2017, "Failed")</f>
+        <f>COUNTIF($I$9:$I$2017, "Failed")</f>
         <v>1</v>
       </c>
     </row>
@@ -5691,7 +5697,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="35">
-        <f>COUNTIF($I$13:$I$2017, "Not Run")</f>
+        <f>COUNTIF($I$9:$I$2017, "Not Run")</f>
         <v>0</v>
       </c>
     </row>
@@ -5707,7 +5713,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="35">
-        <f>COUNTIF($I$13:$I$2017, "Not Completed")</f>
+        <f>COUNTIF($I$9:$I$2017, "Not Completed")</f>
         <v>0</v>
       </c>
     </row>
@@ -5723,41 +5729,41 @@
         <v>29</v>
       </c>
       <c r="I6" s="35">
-        <f>COUNTA(C12:C2016)</f>
-        <v>3</v>
+        <f>COUNTA(C9:C2016)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="125" t="s">
+      <c r="D7" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="141" t="s">
+      <c r="E7" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="142"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="125" t="s">
+      <c r="F7" s="121"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="125" t="s">
+      <c r="I7" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="125" t="s">
+      <c r="J7" s="118" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
+      <c r="B8" s="159"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="159"/>
       <c r="E8" s="17" t="s">
         <v>20</v>
       </c>
@@ -5767,94 +5773,94 @@
       <c r="G8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="159"/>
+      <c r="J8" s="159"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
-      <c r="B9" s="112" t="s">
-        <v>199</v>
-      </c>
-      <c r="C9" s="161" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" s="131" t="s">
+      <c r="B9" s="179" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" s="157" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="109" t="s">
         <v>171</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="F9" s="53" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="G9" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="150" t="s">
-        <v>173</v>
-      </c>
-      <c r="I9" s="155" t="s">
+      <c r="H9" s="156" t="s">
+        <v>172</v>
+      </c>
+      <c r="I9" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="124"/>
+      <c r="J9" s="129"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="113"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="98"/>
+      <c r="B10" s="181"/>
+      <c r="C10" s="158"/>
+      <c r="D10" s="106"/>
       <c r="E10" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="F10" s="53" t="s">
-        <v>172</v>
+        <v>174</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="G10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="165"/>
-      <c r="I10" s="166"/>
-      <c r="J10" s="124"/>
+      <c r="H10" s="172"/>
+      <c r="I10" s="174"/>
+      <c r="J10" s="129"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="113"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="164"/>
+      <c r="B11" s="181"/>
+      <c r="C11" s="158"/>
+      <c r="D11" s="171"/>
       <c r="E11" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="F11" s="53" t="s">
-        <v>172</v>
+        <v>175</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="G11" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="151"/>
-      <c r="I11" s="156"/>
-      <c r="J11" s="124"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="175"/>
+      <c r="J11" s="129"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
-      <c r="B12" s="114"/>
+      <c r="B12" s="180"/>
       <c r="C12" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="D12" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="F12" s="19" t="s">
         <v>178</v>
-      </c>
-      <c r="F12" s="53" t="s">
-        <v>179</v>
       </c>
       <c r="G12" s="66" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I12" s="56" t="s">
         <v>1</v>
@@ -5862,111 +5868,111 @@
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="179" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="186" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="C13" s="112" t="s">
-        <v>197</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E13" s="19" t="s">
+      <c r="F13" s="59" t="s">
         <v>182</v>
-      </c>
-      <c r="F13" s="59" t="s">
-        <v>183</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="163" t="s">
-        <v>184</v>
-      </c>
-      <c r="I13" s="112" t="s">
+      <c r="H13" s="176" t="s">
+        <v>183</v>
+      </c>
+      <c r="I13" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="124"/>
+      <c r="J13" s="129"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="114"/>
-      <c r="C14" s="114"/>
+      <c r="B14" s="180"/>
+      <c r="C14" s="187"/>
       <c r="D14" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>187</v>
-      </c>
       <c r="F14" s="60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G14" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="137"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="124"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="129"/>
     </row>
     <row r="15" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="132" t="s">
-        <v>194</v>
-      </c>
-      <c r="C15" s="121" t="s">
-        <v>198</v>
-      </c>
-      <c r="D15" s="131" t="s">
+      <c r="B15" s="164" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="110" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" s="106" t="s">
         <v>188</v>
       </c>
-      <c r="E15" s="98" t="s">
+      <c r="F15" s="59" t="s">
         <v>189</v>
-      </c>
-      <c r="F15" s="59" t="s">
-        <v>190</v>
       </c>
       <c r="G15" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="168" t="s">
-        <v>193</v>
-      </c>
-      <c r="I15" s="171" t="s">
+      <c r="H15" s="169" t="s">
+        <v>192</v>
+      </c>
+      <c r="I15" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="J15" s="128"/>
+      <c r="J15" s="130"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="132"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="99"/>
+      <c r="B16" s="164"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="107"/>
       <c r="F16" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G16" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="168"/>
-      <c r="I16" s="172"/>
-      <c r="J16" s="128"/>
+      <c r="H16" s="169"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="130"/>
     </row>
     <row r="17" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="132"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="167"/>
-      <c r="E17" s="100"/>
+      <c r="B17" s="164"/>
+      <c r="C17" s="111"/>
+      <c r="D17" s="168"/>
+      <c r="E17" s="108"/>
       <c r="F17" s="60" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G17" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="169"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="129"/>
+      <c r="H17" s="170"/>
+      <c r="I17" s="125"/>
+      <c r="J17" s="131"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -6311,6 +6317,20 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
     <mergeCell ref="J15:J17"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="B15:B17"/>
@@ -6318,20 +6338,6 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="H13:H14"/>
@@ -6353,7 +6359,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6370,17 +6376,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" x14ac:dyDescent="0.5">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="117" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -6394,8 +6400,8 @@
         <v>1</v>
       </c>
       <c r="I2" s="35">
-        <f>COUNTIF($I$14:$I$2018, "Passed")</f>
-        <v>0</v>
+        <f>COUNTIF($I$9:$I$2018, "Passed")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.3">
@@ -6410,8 +6416,8 @@
         <v>2</v>
       </c>
       <c r="I3" s="35">
-        <f>COUNTIF($I$14:$I$2018, "Failed")</f>
-        <v>0</v>
+        <f>COUNTIF($I$9:$I$2018, "Failed")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.3">
@@ -6426,7 +6432,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="35">
-        <f>COUNTIF($I$14:$I$2018, "Not Run")</f>
+        <f>COUNTIF($I$9:$I$2018, "Not Run")</f>
         <v>0</v>
       </c>
     </row>
@@ -6442,7 +6448,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="35">
-        <f>COUNTIF($I$14:$I$2018, "Not Completed")</f>
+        <f>COUNTIF($I$9:$I$2018, "Not Completed")</f>
         <v>0</v>
       </c>
     </row>
@@ -6458,41 +6464,41 @@
         <v>29</v>
       </c>
       <c r="I6" s="35">
-        <f>COUNTA(C12:C2017)</f>
-        <v>1</v>
+        <f>COUNTA(I9:I2025)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="125" t="s">
+      <c r="D7" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="141" t="s">
+      <c r="E7" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="142"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="125" t="s">
+      <c r="F7" s="121"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="125" t="s">
+      <c r="I7" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="125" t="s">
+      <c r="J7" s="118" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
+      <c r="B8" s="159"/>
+      <c r="C8" s="159"/>
+      <c r="D8" s="159"/>
       <c r="E8" s="17" t="s">
         <v>20</v>
       </c>
@@ -6502,117 +6508,117 @@
       <c r="G8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="159"/>
+      <c r="J8" s="159"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
-      <c r="B9" s="177" t="s">
-        <v>221</v>
-      </c>
-      <c r="C9" s="121" t="s">
+      <c r="B9" s="179" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="110" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="106" t="s">
         <v>217</v>
       </c>
-      <c r="D9" s="98" t="s">
-        <v>219</v>
-      </c>
       <c r="E9" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G9" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="164" t="s">
-        <v>230</v>
+      <c r="H9" s="171" t="s">
+        <v>228</v>
       </c>
       <c r="I9" s="183" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="124"/>
+      <c r="J9" s="129"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="179"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="99"/>
+      <c r="B10" s="181"/>
+      <c r="C10" s="116"/>
+      <c r="D10" s="107"/>
       <c r="E10" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="180"/>
+      <c r="H10" s="182"/>
       <c r="I10" s="184"/>
-      <c r="J10" s="124"/>
+      <c r="J10" s="129"/>
     </row>
     <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="178"/>
-      <c r="C11" s="123"/>
-      <c r="D11" s="100"/>
+      <c r="B11" s="180"/>
+      <c r="C11" s="111"/>
+      <c r="D11" s="108"/>
       <c r="E11" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="120"/>
+      <c r="H11" s="150"/>
       <c r="I11" s="185"/>
-      <c r="J11" s="124"/>
+      <c r="J11" s="129"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
-      <c r="B12" s="177" t="s">
+      <c r="B12" s="179" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="112" t="s">
+      <c r="C12" s="100" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" s="106" t="s">
+        <v>225</v>
+      </c>
+      <c r="E12" s="59" t="s">
         <v>226</v>
       </c>
-      <c r="D12" s="98" t="s">
-        <v>227</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>228</v>
-      </c>
       <c r="F12" s="59" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G12" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="181" t="s">
-        <v>232</v>
-      </c>
-      <c r="I12" s="155" t="s">
+      <c r="H12" s="177" t="s">
+        <v>230</v>
+      </c>
+      <c r="I12" s="173" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="178"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="100"/>
+      <c r="B13" s="180"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="108"/>
       <c r="E13" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="F13" s="60" t="s">
         <v>229</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>231</v>
       </c>
       <c r="G13" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="182"/>
-      <c r="I13" s="156"/>
+      <c r="H13" s="178"/>
+      <c r="I13" s="175"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
@@ -6624,7 +6630,7 @@
       <c r="G14" s="36"/>
       <c r="H14" s="22"/>
       <c r="I14" s="43"/>
-      <c r="J14" s="124"/>
+      <c r="J14" s="129"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
@@ -6636,7 +6642,7 @@
       <c r="G15" s="36"/>
       <c r="H15" s="22"/>
       <c r="I15" s="43"/>
-      <c r="J15" s="124"/>
+      <c r="J15" s="129"/>
     </row>
     <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
@@ -6648,7 +6654,7 @@
       <c r="G16" s="36"/>
       <c r="H16" s="22"/>
       <c r="I16" s="43"/>
-      <c r="J16" s="128"/>
+      <c r="J16" s="130"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
@@ -6660,7 +6666,7 @@
       <c r="G17" s="36"/>
       <c r="H17" s="22"/>
       <c r="I17" s="43"/>
-      <c r="J17" s="128"/>
+      <c r="J17" s="130"/>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -6672,7 +6678,7 @@
       <c r="G18" s="36"/>
       <c r="H18" s="22"/>
       <c r="I18" s="43"/>
-      <c r="J18" s="129"/>
+      <c r="J18" s="131"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
@@ -7017,11 +7023,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="J16:J18"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="J14:J15"/>
@@ -7031,13 +7039,11 @@
     <mergeCell ref="H9:H11"/>
     <mergeCell ref="I9:I11"/>
     <mergeCell ref="J9:J11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I34:I50 I21 I25:I26 I28 I31 I19 I15" xr:uid="{10709227-BD79-4859-8427-97CB9B5769EB}">
@@ -7050,18 +7056,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7268,14 +7274,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5836DDC-7C5A-4A10-AADE-992968780C6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6D29AC8-64C8-42E6-B9A9-3FBB4573926C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -7288,6 +7286,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="5d0b22ea-e5ea-49c7-9b62-902e21e51f08"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5836DDC-7C5A-4A10-AADE-992968780C6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>